<commit_message>
changes to data and system prompt
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev02chandan/Documents/Intern@MatiriAI/Property LLM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941A53CB-5D00-EA4E-8A27-FA9C70408DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F14CBC-1BD2-FA41-9243-ACD3CFC872C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="163">
   <si>
     <t>id</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Sleeping Arrangements</t>
-  </si>
-  <si>
-    <t>Important Notes</t>
   </si>
   <si>
     <t>Local Attractions</t>
@@ -237,11 +234,6 @@
  +AE2</t>
   </si>
   <si>
-    <t>FireFly Lawn Care &amp; ...
- -
- +1 865-607-7520</t>
-  </si>
-  <si>
     <t>Standard Departure Clean
  Cleaning
  Mateo Santizo
@@ -573,16 +565,6 @@
  Dispose of bagged and tied trash inside the bear-proof trash bin located in the driveway.</t>
   </si>
   <si>
-    <t>Arrow Exterminators
- -
- +1 865-453-5860
- -
- FireFly Lawn Care &amp; ...
- -
- +1 865-607-7520
- -</t>
-  </si>
-  <si>
     <t>Pack Bag
  Cleaning
  Laundry
@@ -674,51 +656,6 @@
   </si>
   <si>
     <t>The home is conveniently located 10 miles from the parkway in Pigeon Forge and less than 20 miles from the historic charm of downtown Gatlinburg. The property is also just 9 miles from Townsend, offering additional national park access, shops, dining, and river tubing. Famous country singer, Dolly Parton, was born in Sevier County, making it a must-visit for her fans. Dollywood, a theme park jointly owned by Parton, is less than 14 miles from the home. The town and surrounding areas offer a plethora of shopping options, from galleries and boutiques to antique malls and flea markets. Treetop Paradise offers a unique and enjoyable experience, whether you're chasing waterfalls, sampling the best southern BBQ, or simply enjoying your surroundings.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property Name: Treetop Paradise
-Address: 3103 Perry Lane Circle, Sevierville, TN 37862, US
-Description: 1 set of towels (bath towel, hand towel, washcloth) per occupant (up to max occupancy on listing)
- 2 rolls of toilet paper, bar soap or liquid soap dispenser, and wastebasket trash bag per bathroom
- Shampoo, Conditioner, &amp;amp; Body Wash pump bottle per full bathroom
- 2 rolls of paper towels, fresh sponge, dish soap, 3 loads of dishwasher detergent, 3 trash bags per kitchen.
- 3 loads of laundry detergent per home (with in-house laundry systems)
-Max Occupancy: 15.0
-Bedrooms: 3.0, Full Bathrooms: 3.0, Three Quarter Bathrooms: 0.0, Half Bathrooms: 0.0
-Check-in Time: 16:00:00, Check-out Time: 10:00:00, Early Check-in Time: 12:00:00, Late Check-out Time: 15:00:00
-Access: Guest Access Code
- Guest Access Notes
- Parking
- There is parking space provided for up to 4 vehicles in the covered carport, with space for 2-3 more vehicles along the street.
- The entry door is equipped with an electronic lock
- The code will activate right at 4 PM
- To unlock, enter the code provided, the lock will flash green, then turn the deadbolt.
- The door does NOT lock automatically so please lock it when you leave.
- To lock, turn the deadbolt.
- Wifi Name
- ATTfiWRHqs
- Wifi Password
- nd2+i%gzk3n4
- Wifi Notes
- Wifi Router Location
- Main Level | Living Room | Between doors leading outside to deck
-Location: Welcome to Treetop Paradise, aptly named for its elevated positioning among lush greenery. Located in the peaceful Wears Valley area of East Tennessee, this three-story home is perfect for large groups or multiple families. The home is close to local shops, restaurants, wineries, and distilleries and is a stone's throw from the "secret" Metcalf Bottoms entrance to the Great Smoky Mountains National Park.
-Outdoor Features: The main attraction of the property is the wraparound deck with a hot tub, which offers panoramic views of the surrounding landscape. The deck includes a grill and a covered dining area, allowing for outdoor meals with a view.
-Interior Amenities: Inside, the open-concept design and floor-to-ceiling wood furnishings create a cozy, inviting space. The living room features peaked wooden-plank ceilings, a fireplace, and comfortable seating. The fully equipped kitchen comes with a suite of appliances and an island with stools, perfect for prepping meals or casual socializing. A spacious dining table accommodates all guests. The property also boasts a private game room equipped with a pool table, multicade arcade game, wet bar, sofa sleeper, game table, and a twin-over-full bunk bed. The game room opens up to the lower level deck with a hot tub, offering even more entertainment space.
-Sleeping Arrangements: This 3000-square-foot home sleeps up to 15 guests comfortably. It includes three suite-style bedrooms, a loft, and additional beds in the game room. The primary bedroom on the third floor features a king bed, TV, en-suite with a jacuzzi tub and separate shower, and an adjacent private loft with a twin-over-twin bunk bed. The second bedroom on the main floor has a king bed, TV, walk-in closet, and a Jack-and-Jill style bathroom. The third bedroom, on the first floor, features a king bed, closet, and direct access to a full bath.
-Important Notes: 
-Local Attractions: The home is conveniently located 10 miles from the parkway in Pigeon Forge and less than 20 miles from the historic charm of downtown Gatlinburg. The property is also just 9 miles from Townsend, offering additional national park access, shops, dining, and river tubing. Famous country singer, Dolly Parton, was born in Sevier County, making it a must-visit for her fans. Dollywood, a theme park jointly owned by Parton, is less than 14 miles from the home. The town and surrounding areas offer a plethora of shopping options, from galleries and boutiques to antique malls and flea markets. Treetop Paradise offers a unique and enjoyable experience, whether you're chasing waterfalls, sampling the best southern BBQ, or simply enjoying your surroundings.
-Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/Treetop_Paradise-102402-15
-Property Listing on Airbnb: https://www.airbnb.com/rooms/669464604242003293
-Contacts: Arrow Exterminators
- -
- +1 865-453-5860
- -
- FireFly Lawn Care &amp; ...
- -
- +1 865-607-7520
- -
-</t>
   </si>
   <si>
     <t>https://www.grandwelcome.com/vrp/unit/Rays_Chalet-102536-15</t>
@@ -2244,6 +2181,55 @@
 </t>
   </si>
   <si>
+    <t>FireFly Lawn Care  +1 865-607-7520</t>
+  </si>
+  <si>
+    <t>Arrow Exterminators
+ +1 865-453-5860
+ -
+ FireFly Lawn Care &amp; ...
+ -
+ +1 865-607-7520
+ -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Name: Treetop Paradise
+Address: 3103 Perry Lane Circle, Sevierville, TN 37862, US
+Description: 1 set of towels (bath towel, hand towel, washcloth) per occupant (up to max occupancy on listing)
+ 2 rolls of toilet paper, bar soap or liquid soap dispenser, and wastebasket trash bag per bathroom
+ Shampoo, Conditioner, &amp;amp; Body Wash pump bottle per full bathroom
+ 2 rolls of paper towels, fresh sponge, dish soap, 3 loads of dishwasher detergent, 3 trash bags per kitchen.
+ 3 loads of laundry detergent per home (with in-house laundry systems)
+Max Occupancy: 15.0
+Bedrooms: 3.0, Full Bathrooms: 3.0, Three Quarter Bathrooms: 0.0, Half Bathrooms: 0.0
+Check-in Time: 16:00:00, Check-out Time: 10:00:00, Early Check-in Time: 12:00:00, Late Check-out Time: 15:00:00
+Access: Guest Access Code
+ Guest Access Notes
+ Parking
+ There is parking space provided for up to 4 vehicles in the covered carport, with space for 2-3 more vehicles along the street.
+ The entry door is equipped with an electronic lock
+ The code will activate right at 4 PM
+ To unlock, enter the code provided, the lock will flash green, then turn the deadbolt.
+ The door does NOT lock automatically so please lock it when you leave.
+ To lock, turn the deadbolt.
+ Wifi Name
+ ATTfiWRHqs
+ Wifi Password
+ nd2+i%gzk3n4
+ Wifi Notes
+ Wifi Router Location
+ Main Level | Living Room | Between doors leading outside to deck
+Location: Welcome to Treetop Paradise, aptly named for its elevated positioning among lush greenery. Located in the peaceful Wears Valley area of East Tennessee, this three-story home is perfect for large groups or multiple families. The home is close to local shops, restaurants, wineries, and distilleries and is a stone's throw from the "secret" Metcalf Bottoms entrance to the Great Smoky Mountains National Park.
+Outdoor Features: The main attraction of the property is the wraparound deck with a hot tub, which offers panoramic views of the surrounding landscape. The deck includes a grill and a covered dining area, allowing for outdoor meals with a view.
+Interior Amenities: Inside, the open-concept design and floor-to-ceiling wood furnishings create a cozy, inviting space. The living room features peaked wooden-plank ceilings, a fireplace, and comfortable seating. The fully equipped kitchen comes with a suite of appliances and an island with stools, perfect for prepping meals or casual socializing. A spacious dining table accommodates all guests. The property also boasts a private game room equipped with a pool table, multicade arcade game, wet bar, sofa sleeper, game table, and a twin-over-full bunk bed. The game room opens up to the lower level deck with a hot tub, offering even more entertainment space.
+Sleeping Arrangements: This 3000-square-foot home sleeps up to 15 guests comfortably. It includes three suite-style bedrooms, a loft, and additional beds in the game room. The primary bedroom on the third floor features a king bed, TV, en-suite with a jacuzzi tub and separate shower, and an adjacent private loft with a twin-over-twin bunk bed. The second bedroom on the main floor has a king bed, TV, walk-in closet, and a Jack-and-Jill style bathroom. The third bedroom, on the first floor, features a king bed, closet, and direct access to a full bath.
+Important Notes: 
+Local Attractions: The home is conveniently located 10 miles from the parkway in Pigeon Forge and less than 20 miles from the historic charm of downtown Gatlinburg. The property is also just 9 miles from Townsend, offering additional national park access, shops, dining, and river tubing. Famous country singer, Dolly Parton, was born in Sevier County, making it a must-visit for her fans. Dollywood, a theme park jointly owned by Parton, is less than 14 miles from the home. The town and surrounding areas offer a plethora of shopping options, from galleries and boutiques to antique malls and flea markets. Treetop Paradise offers a unique and enjoyable experience, whether you're chasing waterfalls, sampling the best southern BBQ, or simply enjoying your surroundings.
+Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/Treetop_Paradise-102402-15
+Property Listing on Airbnb: https://www.airbnb.com/rooms/669464604242003293
+Contacts: Arrow Exterminators +1 865-453-5860 ,  +1 865-607-7520 (FireFly Lawn Care) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Name: The Real McCoy
 Address: 2424 Walnut Ridge Way, Sevierville, TN 37862, US
 Description: 1 set of towels (bath towel, hand towel, washcloth) per occupant (up to max occupancy on listing)
@@ -2275,7 +2261,7 @@
 Local Attractions: The home's location in Sevierville is a notable birthplace of country singer Dolly Parton, and the family theme park Dollywood, jointly owned by Parton, is located under 10 miles from the home. For shopping enthusiasts, the town and surrounding areas are filled with galleries, boutiques, antique malls, flea markets, and more! Whether you're chasing waterfalls, tasting the best southern BBQ, or just exploring on a whim, you're sure to make unforgettable memories in Sevierville!
 Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/The_Real_McCoy-102369-15
 Property Listing on Airbnb: https://www.airbnb.com/rooms/658522003554413078
-Contacts: FireFly Lawn Care -  +1 865-607-7520
+Contacts for any issue:  +1 865-607-7520 (FireFly Lawn Care) 
 </t>
   </si>
 </sst>
@@ -2643,18 +2629,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="36" max="36" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="89.83203125" customWidth="1"/>
+    <col min="26" max="26" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="63.33203125" customWidth="1"/>
+    <col min="28" max="28" width="32" customWidth="1"/>
+    <col min="29" max="29" width="48.6640625" customWidth="1"/>
+    <col min="30" max="30" width="35.33203125" customWidth="1"/>
+    <col min="31" max="31" width="43.1640625" customWidth="1"/>
+    <col min="32" max="32" width="62" customWidth="1"/>
+    <col min="33" max="33" width="42.6640625" customWidth="1"/>
+    <col min="34" max="34" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2760,861 +2764,858 @@
       <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1512</v>
+      </c>
+      <c r="B2" s="2">
+        <v>102369</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="2">
+        <v>37862</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2360</v>
+      </c>
+      <c r="M2" s="2">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2">
+        <v>3</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="2">
+        <v>-83.608500000000006</v>
+      </c>
+      <c r="T2" s="2">
+        <v>35.75112</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1512</v>
-      </c>
-      <c r="B2">
-        <v>102369</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1545</v>
+      </c>
+      <c r="B3" s="2">
+        <v>102402</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J3" s="2">
+        <v>37862</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J2">
+      <c r="L3" s="2">
+        <v>3020</v>
+      </c>
+      <c r="M3" s="2">
+        <v>15</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3</v>
+      </c>
+      <c r="O3" s="2">
+        <v>3</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="2">
+        <v>-83.617900000000006</v>
+      </c>
+      <c r="T3" s="2">
+        <v>35.713079999999998</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1679</v>
+      </c>
+      <c r="B4" s="2">
+        <v>102536</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="2">
+        <v>37876</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="2">
+        <v>800</v>
+      </c>
+      <c r="M4" s="2">
+        <v>6</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="2">
+        <v>-83.414299999999997</v>
+      </c>
+      <c r="T4" s="2">
+        <v>35.793480000000002</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1849</v>
+      </c>
+      <c r="B5" s="2">
+        <v>102706</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="2">
         <v>37862</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3000</v>
+      </c>
+      <c r="M5" s="2">
+        <v>15</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5</v>
+      </c>
+      <c r="O5" s="2">
+        <v>4</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L2">
-        <v>2360</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
+      <c r="S5" s="2">
+        <v>-83.663300000000007</v>
+      </c>
+      <c r="T5" s="2">
+        <v>35.779809999999998</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>1899</v>
+      </c>
+      <c r="B6" s="2">
+        <v>102756</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="2">
+        <v>37862</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="2">
+        <v>4</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="2">
+        <v>-83.608000000000004</v>
+      </c>
+      <c r="T6" s="2">
+        <v>35.814050000000002</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>1900</v>
+      </c>
+      <c r="B7" s="2">
+        <v>102757</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="2">
+        <v>37862</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M7" s="2">
+        <v>7</v>
+      </c>
+      <c r="N7" s="2">
+        <v>2</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="2">
+        <v>-83.608000000000004</v>
+      </c>
+      <c r="T7" s="2">
+        <v>35.814050000000002</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>1901</v>
+      </c>
+      <c r="B8" s="2">
+        <v>102758</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="2">
+        <v>37862</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="2">
+        <v>11</v>
+      </c>
+      <c r="N8" s="2">
+        <v>4</v>
+      </c>
+      <c r="O8" s="2">
+        <v>4</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="2">
+        <v>-83.608000000000004</v>
+      </c>
+      <c r="T8" s="2">
+        <v>35.814050000000002</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" s="2" customFormat="1" ht="405" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B9" s="2">
+        <v>102853</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="2">
+        <v>37876</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="2">
+        <v>2063</v>
+      </c>
+      <c r="M9" s="2">
+        <v>8</v>
+      </c>
+      <c r="N9" s="2">
+        <v>4</v>
+      </c>
+      <c r="O9" s="2">
         <v>3</v>
       </c>
-      <c r="O2">
-        <v>3</v>
-      </c>
-      <c r="P2">
+      <c r="P9" s="2">
         <v>0</v>
       </c>
-      <c r="Q2">
+      <c r="Q9" s="2">
         <v>0</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="2">
+        <v>-83.5227</v>
+      </c>
+      <c r="T9" s="2">
+        <v>35.810099999999998</v>
+      </c>
+      <c r="U9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S2">
-        <v>-83.608500000000006</v>
-      </c>
-      <c r="T2">
-        <v>35.75112</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="X2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1545</v>
-      </c>
-      <c r="B3">
-        <v>102402</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3">
-        <v>37862</v>
-      </c>
-      <c r="K3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3">
-        <v>3020</v>
-      </c>
-      <c r="M3">
-        <v>15</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3">
-        <v>3</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3">
-        <v>-83.617900000000006</v>
-      </c>
-      <c r="T3">
-        <v>35.713079999999998</v>
-      </c>
-      <c r="U3" t="s">
-        <v>45</v>
-      </c>
-      <c r="V3" t="s">
-        <v>46</v>
-      </c>
-      <c r="W3" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1679</v>
-      </c>
-      <c r="B4">
-        <v>102536</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4">
-        <v>37876</v>
-      </c>
-      <c r="K4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4">
-        <v>800</v>
-      </c>
-      <c r="M4">
-        <v>6</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4">
-        <v>-83.414299999999997</v>
-      </c>
-      <c r="T4">
-        <v>35.793480000000002</v>
-      </c>
-      <c r="U4" t="s">
-        <v>45</v>
-      </c>
-      <c r="V4" t="s">
-        <v>46</v>
-      </c>
-      <c r="W4" t="s">
-        <v>47</v>
-      </c>
-      <c r="X4" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1849</v>
-      </c>
-      <c r="B5">
-        <v>102706</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5">
-        <v>37862</v>
-      </c>
-      <c r="K5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5">
-        <v>3000</v>
-      </c>
-      <c r="M5">
-        <v>15</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5" t="s">
-        <v>44</v>
-      </c>
-      <c r="S5">
-        <v>-83.663300000000007</v>
-      </c>
-      <c r="T5">
-        <v>35.779809999999998</v>
-      </c>
-      <c r="U5" t="s">
-        <v>45</v>
-      </c>
-      <c r="V5" t="s">
-        <v>46</v>
-      </c>
-      <c r="W5" t="s">
-        <v>47</v>
-      </c>
-      <c r="X5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1899</v>
-      </c>
-      <c r="B6">
-        <v>102756</v>
-      </c>
-      <c r="C6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6">
-        <v>37862</v>
-      </c>
-      <c r="K6" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6">
-        <v>1000</v>
-      </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
-      <c r="N6">
-        <v>2</v>
-      </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
-        <v>44</v>
-      </c>
-      <c r="S6">
-        <v>-83.608000000000004</v>
-      </c>
-      <c r="T6">
-        <v>35.814050000000002</v>
-      </c>
-      <c r="U6" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" t="s">
-        <v>46</v>
-      </c>
-      <c r="W6" t="s">
-        <v>47</v>
-      </c>
-      <c r="X6" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1900</v>
-      </c>
-      <c r="B7">
-        <v>102757</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7">
-        <v>37862</v>
-      </c>
-      <c r="K7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7">
-        <v>2000</v>
-      </c>
-      <c r="M7">
-        <v>7</v>
-      </c>
-      <c r="N7">
-        <v>2</v>
-      </c>
-      <c r="O7">
-        <v>2</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7">
-        <v>-83.608000000000004</v>
-      </c>
-      <c r="T7">
-        <v>35.814050000000002</v>
-      </c>
-      <c r="U7" t="s">
-        <v>45</v>
-      </c>
-      <c r="V7" t="s">
-        <v>46</v>
-      </c>
-      <c r="W7" t="s">
-        <v>47</v>
-      </c>
-      <c r="X7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>123</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1901</v>
-      </c>
-      <c r="B8">
-        <v>102758</v>
-      </c>
-      <c r="C8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8">
-        <v>37862</v>
-      </c>
-      <c r="K8" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8">
-        <v>1000</v>
-      </c>
-      <c r="M8">
-        <v>11</v>
-      </c>
-      <c r="N8">
-        <v>4</v>
-      </c>
-      <c r="O8">
-        <v>4</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>44</v>
-      </c>
-      <c r="S8">
-        <v>-83.608000000000004</v>
-      </c>
-      <c r="T8">
-        <v>35.814050000000002</v>
-      </c>
-      <c r="U8" t="s">
-        <v>45</v>
-      </c>
-      <c r="V8" t="s">
-        <v>46</v>
-      </c>
-      <c r="W8" t="s">
-        <v>47</v>
-      </c>
-      <c r="X8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>144</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1996</v>
-      </c>
-      <c r="B9">
-        <v>102853</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="Y9" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D9" t="s">
+      <c r="Z9" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="AA9" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G9" t="s">
+      <c r="AB9" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9">
-        <v>37876</v>
-      </c>
-      <c r="K9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9">
-        <v>2063</v>
-      </c>
-      <c r="M9">
-        <v>8</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>44</v>
-      </c>
-      <c r="S9">
-        <v>-83.5227</v>
-      </c>
-      <c r="T9">
-        <v>35.810099999999998</v>
-      </c>
-      <c r="U9" t="s">
-        <v>45</v>
-      </c>
-      <c r="V9" t="s">
-        <v>46</v>
-      </c>
-      <c r="W9" t="s">
-        <v>47</v>
-      </c>
-      <c r="X9" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y9" t="s">
+      <c r="AC9" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AD9" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AE9" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AF9" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AG9" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AH9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AI9" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>161</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>